<commit_message>
Modify POM for form Page
</commit_message>
<xml_diff>
--- a/formPage/TestCase-Form-E2E.xlsx
+++ b/formPage/TestCase-Form-E2E.xlsx
@@ -191,26 +191,25 @@
     <t>Fail</t>
   </si>
   <si>
+    <t>firstName='Kha'
+lastName='Hoai'
+gender='Male'
+mobileNumber='9825467895'
+dayOfBirth = '7/2/2003'
+subject = 'Math' 'Chemistry'</t>
+  </si>
+  <si>
+    <t>Verify that student can not register with Moblie Number &lt;  10 digits</t>
+  </si>
+  <si>
     <t>1. Open browser
 2. Visit the website: "https://demoqa.com/automation-practice-form"
 3. Input valid first name: 'Kha'
 4. Input valid last name: 'Hoai'
 5. Select Gender option: 'Male'
 6.Input valid mobile number: '9825467895'
-7. Select valid birthday: '7/2/2003'
-8. Input valid subject: 'Math' 'Chemistry'
-9. Click on Submit button</t>
-  </si>
-  <si>
-    <t>firstName='Kha'
-lastName='Hoai'
-gender='Male'
-mobileNumber='9825467895'
-dayOfBirth = '7/2/2003'
-subject = 'Math' 'Chemistry'</t>
-  </si>
-  <si>
-    <t>Verify that student can not register with Moblie Number &lt;  10 digits</t>
+7. Input valid subject: 'Math' 'Chemistry'
+8. Click on Submit button</t>
   </si>
 </sst>
 </file>
@@ -488,8 +487,8 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>3119439</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>1971500</xdr:rowOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>173656</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -975,8 +974,8 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1023,7 +1022,7 @@
       </c>
       <c r="J1" s="16"/>
     </row>
-    <row r="2" spans="1:10" ht="157.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="str">
         <f>"TC"&amp;ROW()-1</f>
         <v>TC1</v>
@@ -1035,10 +1034,10 @@
         <v>19</v>
       </c>
       <c r="D2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>9</v>
@@ -1155,7 +1154,7 @@
       </c>
       <c r="B7" s="22"/>
       <c r="C7" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>25</v>

</xml_diff>